<commit_message>
Did the first test plan for the Client Class.
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_client.xlsx
+++ b/tests/A01_pixell_test_plan_client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkwarkentin\Documents\Course Folders\2-Intermediate Software Development\Code\Assignments 2024 Spring\Assignment 1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4928f0ddc5ce2e2f/Documents/Red River College/2-Fall 2024/2. Intermediate Software Development/Project/isd_project/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2981098F-0A24-4280-A1E3-2323AE4832DC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Software Development Team - Unit Test Plan</t>
   </si>
@@ -264,13 +264,67 @@
   </si>
   <si>
     <t>Add more rows as necessary</t>
+  </si>
+  <si>
+    <t>Raven Manalastas</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>attributes are set to input values</t>
+  </si>
+  <si>
+    <t>client_number: 7910
+first_name: Jorel
+last_name: Cruz
+email_address: jorelcruz@rrc.ca</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>client_number: 7910
+first_name: ""
+last_name: Curz
+email_address:jorelcruz@rrc.ca</t>
+  </si>
+  <si>
+    <t>client_number: 7910
+first_name: Jorel
+last_name: ""
+email_address: jorelcruz@rrc.ca</t>
+  </si>
+  <si>
+    <t>client_number: 7910
+first_name: Jorel
+last_name: Cruz
+email_address: "jorelcruzrrc.ca"</t>
+  </si>
+  <si>
+    <t>client_number: "INVALID"
+first_name: Jorel
+last_name: Cruz
+email_address: jorelcruz@rrc.ca</t>
+  </si>
+  <si>
+    <t>Jorel</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>jorelcruz@rrc.ca</t>
+  </si>
+  <si>
+    <t>Cruz, Jorel [7910] - jorelcruz@rrc.ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +385,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -504,10 +566,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -558,8 +621,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1087,20 +1157,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.109375" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="7" max="7" width="33.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="1.8">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1112,14 +1184,16 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>27</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1128,10 +1202,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1151,7 +1225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="66" customHeight="1">
+    <row r="7" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="9">
         <v>1</v>
@@ -1162,11 +1236,17 @@
       <c r="D7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="66" customHeight="1">
+      <c r="E7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="11">
         <v>2</v>
@@ -1177,11 +1257,17 @@
       <c r="D8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="66" customHeight="1">
+      <c r="E8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="11">
         <v>3</v>
@@ -1192,11 +1278,17 @@
       <c r="D9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="66" customHeight="1">
+      <c r="E9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="9">
         <v>4</v>
@@ -1207,11 +1299,17 @@
       <c r="D10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="66" customHeight="1">
+      <c r="E10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="11">
         <v>5</v>
@@ -1222,11 +1320,17 @@
       <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="31.15" customHeight="1">
+      <c r="E11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1236,11 +1340,17 @@
       <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="31.15" customHeight="1">
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="20">
+        <v>7910</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>7</v>
       </c>
@@ -1250,11 +1360,17 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1">
+      <c r="E13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1264,11 +1380,17 @@
       <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1">
+      <c r="E14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1278,11 +1400,17 @@
       <c r="D15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1">
+      <c r="E15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>10</v>
       </c>
@@ -1292,11 +1420,17 @@
       <c r="D16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1">
+      <c r="E16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1306,7 +1440,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1">
+    <row r="18" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1316,7 +1450,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1">
+    <row r="19" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>13</v>
       </c>
@@ -1326,7 +1460,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1">
+    <row r="20" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <v>14</v>
       </c>
@@ -1336,7 +1470,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1">
+    <row r="21" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1346,7 +1480,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1">
+    <row r="22" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>16</v>
       </c>
@@ -1356,7 +1490,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1">
+    <row r="23" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <v>17</v>
       </c>
@@ -1366,7 +1500,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1">
+    <row r="24" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1376,7 +1510,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1">
+    <row r="25" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
         <v>19</v>
       </c>
@@ -1386,7 +1520,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1">
+    <row r="26" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11">
         <v>20</v>
       </c>
@@ -1396,7 +1530,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1">
+    <row r="27" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1406,7 +1540,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1">
+    <row r="28" spans="2:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9">
         <v>22</v>
       </c>
@@ -1416,7 +1550,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="19" t="s">
         <v>26</v>
       </c>
@@ -1433,10 +1567,13 @@
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B30:G30"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="G15" r:id="rId1" xr:uid="{BE2D99FB-79E3-46BB-B710-ADB67F4806B4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added BankAccount class with attributes, accessors, and methods for managing bank accounts, including deposit, withdraw, and string representation.
</commit_message>
<xml_diff>
--- a/tests/A01_pixell_test_plan_client.xlsx
+++ b/tests/A01_pixell_test_plan_client.xlsx
@@ -597,6 +597,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -620,12 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -758,6 +758,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1157,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,31 +1180,31 @@
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="18"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
@@ -1346,7 +1350,7 @@
       <c r="F12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="12">
         <v>7910</v>
       </c>
     </row>
@@ -1366,7 +1370,7 @@
       <c r="F13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1386,7 +1390,7 @@
       <c r="F14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1406,7 +1410,7 @@
       <c r="F15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="21" t="s">
+      <c r="G15" s="13" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1426,7 +1430,7 @@
       <c r="F16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="12" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1551,14 +1555,14 @@
       <c r="G28" s="3"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>